<commit_message>
Bar Scan Works Somehow
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="200">
   <si>
     <t>S No</t>
   </si>
@@ -766,6 +766,18 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>02-Oct-2020 11:35</t>
+  </si>
+  <si>
+    <t>150.0</t>
+  </si>
+  <si>
+    <t>XX02104</t>
+  </si>
+  <si>
+    <t>yyy</t>
   </si>
 </sst>
 </file>
@@ -1356,11 +1368,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1372,7 +1384,7 @@
     <col min="6" max="6" width="13.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1392,7 +1404,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1403,10 +1415,10 @@
         <v>4950</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1417,10 +1429,10 @@
         <v>7650</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1431,10 +1443,10 @@
         <v>8850</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="69.95" customHeight="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="69.95" customHeight="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1451,7 +1463,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="69.95" customHeight="1">
+    <row r="6" spans="1:7" ht="69.95" customHeight="1">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1462,13 +1474,16 @@
         <v>100</v>
       </c>
       <c r="D6">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="69.95" customHeight="1">
+      <c r="G6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="69.95" customHeight="1">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1482,7 +1497,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1496,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1507,10 +1522,10 @@
         <v>27000</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="69.95" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="69.95" customHeight="1">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1521,10 +1536,10 @@
         <v>40500</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1538,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1552,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1566,7 +1581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1580,7 +1595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1594,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2247,7 +2262,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2856,6 +2871,29 @@
         <v>193</v>
       </c>
       <c r="G26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F27" t="s">
+        <v>198</v>
+      </c>
+      <c r="G27" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create New Stock and Update Stock Done
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="225">
   <si>
     <t>S No</t>
   </si>
@@ -832,6 +832,27 @@
   </si>
   <si>
     <t>Aqua Fresh(8)</t>
+  </si>
+  <si>
+    <t>Irfaan</t>
+  </si>
+  <si>
+    <t>22222222222</t>
+  </si>
+  <si>
+    <t>Remote2222</t>
+  </si>
+  <si>
+    <t>765765765</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>Apple iPhone</t>
+  </si>
+  <si>
+    <t>321654987</t>
   </si>
 </sst>
 </file>
@@ -906,7 +927,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -928,7 +949,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -966,7 +987,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1004,7 +1025,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:blip r:embed="rId3" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1042,7 +1063,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:blip r:embed="rId4" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1080,7 +1101,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:blip r:embed="rId5" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1118,7 +1139,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:blip r:embed="rId6" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1127,6 +1148,82 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="3638550" cy="841534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3648075</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>841533</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3648075" cy="841534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3648075</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>841533</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3648075" cy="841534"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1423,11 +1520,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1458,6 +1555,9 @@
       <c r="F1" s="5" t="s">
         <v>187</v>
       </c>
+      <c r="G1" s="5" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
@@ -1511,8 +1611,8 @@
       <c r="C5" s="3">
         <v>100</v>
       </c>
-      <c r="D5" t="n">
-        <v>1488.0</v>
+      <c r="D5">
+        <v>1488</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>195</v>
@@ -1529,7 +1629,7 @@
         <v>100</v>
       </c>
       <c r="D6" t="n">
-        <v>139.0</v>
+        <v>250.0</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>194</v>
@@ -1548,8 +1648,8 @@
       <c r="C7" s="3">
         <v>200</v>
       </c>
-      <c r="D7" t="n">
-        <v>1996.0</v>
+      <c r="D7">
+        <v>1996</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1576,8 +1676,8 @@
       <c r="C9" s="3">
         <v>27000</v>
       </c>
-      <c r="D9">
-        <v>100</v>
+      <c r="D9" t="n">
+        <v>300.0</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="69.95" customHeight="1">
@@ -2126,7 +2226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2140,7 +2240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2154,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75">
+    <row r="51" spans="1:6" ht="15.75">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2168,7 +2268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75">
+    <row r="52" spans="1:6" ht="15.75">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2182,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75">
+    <row r="53" spans="1:6" ht="15.75">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2196,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75">
+    <row r="54" spans="1:6" ht="15.75">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2210,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75">
+    <row r="55" spans="1:6" ht="15.75">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2224,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75">
+    <row r="56" spans="1:6" ht="15.75">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2238,7 +2338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75">
+    <row r="57" spans="1:6" ht="15.75">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2252,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75">
+    <row r="58" spans="1:6" ht="15.75">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2266,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75">
+    <row r="59" spans="1:6" ht="15.75">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2280,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75">
+    <row r="60" spans="1:6" ht="15.75">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2294,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75">
+    <row r="61" spans="1:6" ht="15.75">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2306,6 +2406,60 @@
       </c>
       <c r="D61">
         <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="69.95" customHeight="1">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>218</v>
+      </c>
+      <c r="C62">
+        <v>36</v>
+      </c>
+      <c r="D62">
+        <v>100</v>
+      </c>
+      <c r="F62" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>220</v>
+      </c>
+      <c r="C63">
+        <v>55</v>
+      </c>
+      <c r="D63">
+        <v>100</v>
+      </c>
+      <c r="F63" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" ht="70.0" customHeight="true">
+      <c r="A64" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>223</v>
+      </c>
+      <c r="C64" t="n">
+        <v>2500.0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>224</v>
+      </c>
+      <c r="G64" t="n">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>
@@ -2317,7 +2471,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2952,7 +3106,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>200</v>
       </c>
@@ -2975,7 +3129,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>203</v>
       </c>
@@ -2998,7 +3152,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>205</v>
       </c>
@@ -3021,7 +3175,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>205</v>
       </c>
@@ -3044,7 +3198,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>208</v>
       </c>
@@ -3067,7 +3221,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>211</v>
       </c>
@@ -3090,7 +3244,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>213</v>
       </c>
@@ -3113,7 +3267,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>215</v>
       </c>

</xml_diff>

<commit_message>
Yes / No Done
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="161">
   <si>
     <t>S No</t>
   </si>
@@ -362,6 +362,144 @@
   </si>
   <si>
     <t>Stock Name Three(1)</t>
+  </si>
+  <si>
+    <t>02-Dec-2020 14:09</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>XX021284</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>XX021285</t>
+  </si>
+  <si>
+    <t>cutting(1)</t>
+  </si>
+  <si>
+    <t>02-Dec-2020 14:11</t>
+  </si>
+  <si>
+    <t>Sak 2(1)</t>
+  </si>
+  <si>
+    <t>02-Dec-2020 14:22</t>
+  </si>
+  <si>
+    <t>XX021286</t>
+  </si>
+  <si>
+    <t>sakthi masala(1)</t>
+  </si>
+  <si>
+    <t>02-Dec-2020 14:25</t>
+  </si>
+  <si>
+    <t>02-Dec-2020 14:26</t>
+  </si>
+  <si>
+    <t>685</t>
+  </si>
+  <si>
+    <t>sakthi masala(1),Bill Clearance 02Dec2020(1)</t>
+  </si>
+  <si>
+    <t>02-Dec-2020 14:32</t>
+  </si>
+  <si>
+    <t>1600</t>
+  </si>
+  <si>
+    <t>XX021287</t>
+  </si>
+  <si>
+    <t>CP(2)</t>
+  </si>
+  <si>
+    <t>2250</t>
+  </si>
+  <si>
+    <t>CP(2),Bill Clearance 02Dec2020(1)</t>
+  </si>
+  <si>
+    <t>02-Dec-2020 14:34</t>
+  </si>
+  <si>
+    <t>2400</t>
+  </si>
+  <si>
+    <t>1600.0</t>
+  </si>
+  <si>
+    <t>XX021288</t>
+  </si>
+  <si>
+    <t>CP(3)</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>XX021289</t>
+  </si>
+  <si>
+    <t>Sak 2(2)</t>
+  </si>
+  <si>
+    <t>02-Dec-2020 14:35</t>
+  </si>
+  <si>
+    <t>XX021290</t>
+  </si>
+  <si>
+    <t>Sak 2(5)</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>XX021291</t>
+  </si>
+  <si>
+    <t>CP(1)</t>
+  </si>
+  <si>
+    <t>02-Dec-2020 14:39</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>40.0</t>
+  </si>
+  <si>
+    <t>Single Motta (4)</t>
+  </si>
+  <si>
+    <t>XX021292</t>
+  </si>
+  <si>
+    <t>02-Dec-2020 14:40</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>XX021293</t>
+  </si>
+  <si>
+    <t>Stock Name One(1)</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>Stock Name One(1),Bill Clearance 02Dec2020(1)</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1213,8 @@
       <c r="C2" s="3">
         <v>155</v>
       </c>
-      <c r="D2">
-        <v>202</v>
+      <c r="D2" t="n">
+        <v>201.0</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>47</v>
@@ -1119,7 +1257,7 @@
         <v>1000</v>
       </c>
       <c r="D4" t="n">
-        <v>55.0</v>
+        <v>54.0</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>52</v>
@@ -1161,8 +1299,8 @@
       <c r="C6">
         <v>800</v>
       </c>
-      <c r="D6">
-        <v>103</v>
+      <c r="D6" t="n">
+        <v>98.0</v>
       </c>
       <c r="F6" t="s">
         <v>56</v>
@@ -1201,8 +1339,8 @@
       <c r="C8">
         <v>35</v>
       </c>
-      <c r="D8">
-        <v>1</v>
+      <c r="D8" t="n">
+        <v>0.0</v>
       </c>
       <c r="F8" t="s">
         <v>60</v>
@@ -1221,8 +1359,8 @@
       <c r="C9">
         <v>35</v>
       </c>
-      <c r="D9">
-        <v>157</v>
+      <c r="D9" t="n">
+        <v>148.0</v>
       </c>
       <c r="F9" t="s">
         <v>60</v>
@@ -1262,7 +1400,7 @@
         <v>35</v>
       </c>
       <c r="D11" t="n">
-        <v>45.0</v>
+        <v>41.0</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
@@ -1354,7 +1492,7 @@
         <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
         <v>102</v>
@@ -1423,13 +1561,381 @@
         <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F6" t="s">
         <v>113</v>
       </c>
       <c r="G6" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
+        <v>148</v>
+      </c>
+      <c r="G18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>148</v>
+      </c>
+      <c r="G19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>154</v>
+      </c>
+      <c r="G20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" t="s">
+        <v>157</v>
+      </c>
+      <c r="G21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>159</v>
+      </c>
+      <c r="E22" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" t="s">
+        <v>157</v>
+      </c>
+      <c r="G22" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change qty bug Fixed
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="495">
   <si>
     <t>S No</t>
   </si>
@@ -1478,6 +1478,30 @@
   </si>
   <si>
     <t>XX0912145</t>
+  </si>
+  <si>
+    <t>10-Dec-2020 13:38</t>
+  </si>
+  <si>
+    <t>455.0</t>
+  </si>
+  <si>
+    <t>XX1012146</t>
+  </si>
+  <si>
+    <t>Stock Name two(5)</t>
+  </si>
+  <si>
+    <t>10-Dec-2020 13:44</t>
+  </si>
+  <si>
+    <t>XX1012147</t>
+  </si>
+  <si>
+    <t>1255</t>
+  </si>
+  <si>
+    <t>Stock Name two(5),Bill Clearance 10Dec2020(1)</t>
   </si>
 </sst>
 </file>
@@ -2025,7 +2049,7 @@
         <v>200</v>
       </c>
       <c r="D3" t="n">
-        <v>435.0</v>
+        <v>425.0</v>
       </c>
       <c r="F3" t="s">
         <v>164</v>
@@ -5032,7 +5056,7 @@
         <v>428</v>
       </c>
       <c r="E128" t="s">
-        <v>35</v>
+        <v>345</v>
       </c>
       <c r="F128" t="s">
         <v>426</v>
@@ -5430,6 +5454,75 @@
       </c>
       <c r="G145" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>487</v>
+      </c>
+      <c r="B146" t="s">
+        <v>98</v>
+      </c>
+      <c r="C146" t="s">
+        <v>99</v>
+      </c>
+      <c r="D146" t="s">
+        <v>227</v>
+      </c>
+      <c r="E146" t="s">
+        <v>345</v>
+      </c>
+      <c r="F146" t="s">
+        <v>489</v>
+      </c>
+      <c r="G146" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>491</v>
+      </c>
+      <c r="B147" t="s">
+        <v>98</v>
+      </c>
+      <c r="C147" t="s">
+        <v>99</v>
+      </c>
+      <c r="D147" t="s">
+        <v>111</v>
+      </c>
+      <c r="E147" t="s">
+        <v>345</v>
+      </c>
+      <c r="F147" t="s">
+        <v>492</v>
+      </c>
+      <c r="G147" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>491</v>
+      </c>
+      <c r="B148" t="s">
+        <v>98</v>
+      </c>
+      <c r="C148" t="s">
+        <v>99</v>
+      </c>
+      <c r="D148" t="s">
+        <v>493</v>
+      </c>
+      <c r="E148" t="s">
+        <v>35</v>
+      </c>
+      <c r="F148" t="s">
+        <v>492</v>
+      </c>
+      <c r="G148" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Double Bill Issue Fixed
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="521">
   <si>
     <t>S No</t>
   </si>
@@ -1514,6 +1514,72 @@
   </si>
   <si>
     <t>654</t>
+  </si>
+  <si>
+    <t>15-Dec-2020 09:58</t>
+  </si>
+  <si>
+    <t>675.0</t>
+  </si>
+  <si>
+    <t>XX1512148</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>XX1512149</t>
+  </si>
+  <si>
+    <t>New Liz(1)</t>
+  </si>
+  <si>
+    <t>690</t>
+  </si>
+  <si>
+    <t>New Liz(1),Bill Clearance 15Dec2020(1)</t>
+  </si>
+  <si>
+    <t>15-Dec-2020 10:06</t>
+  </si>
+  <si>
+    <t>4600</t>
+  </si>
+  <si>
+    <t>4450.0</t>
+  </si>
+  <si>
+    <t>XX1512150</t>
+  </si>
+  <si>
+    <t>Stock Name two(23)</t>
+  </si>
+  <si>
+    <t>XX1512151</t>
+  </si>
+  <si>
+    <t>15-Dec-2020 10:10</t>
+  </si>
+  <si>
+    <t>3410</t>
+  </si>
+  <si>
+    <t>3310.0</t>
+  </si>
+  <si>
+    <t>Stock Name One(22)</t>
+  </si>
+  <si>
+    <t>XX1512152</t>
+  </si>
+  <si>
+    <t>Newss Sss(1)</t>
+  </si>
+  <si>
+    <t>3460</t>
+  </si>
+  <si>
+    <t>Newss Sss(1),Bill Clearance 15Dec2020(1)</t>
   </si>
 </sst>
 </file>
@@ -2038,7 +2104,7 @@
         <v>155</v>
       </c>
       <c r="D2" t="n">
-        <v>166.0</v>
+        <v>139.0</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>157</v>
@@ -2061,7 +2127,7 @@
         <v>200</v>
       </c>
       <c r="D3" t="n">
-        <v>425.0</v>
+        <v>402.0</v>
       </c>
       <c r="F3" t="s">
         <v>164</v>
@@ -2121,7 +2187,7 @@
         <v>150.0</v>
       </c>
       <c r="D6" t="n">
-        <v>100.0</v>
+        <v>99.0</v>
       </c>
       <c r="F6" t="s">
         <v>496</v>
@@ -2141,7 +2207,7 @@
         <v>15.0</v>
       </c>
       <c r="D7" t="n">
-        <v>200.0</v>
+        <v>199.0</v>
       </c>
       <c r="F7" t="s">
         <v>498</v>
@@ -5476,7 +5542,7 @@
         <v>481</v>
       </c>
       <c r="E144" t="s">
-        <v>35</v>
+        <v>345</v>
       </c>
       <c r="F144" t="s">
         <v>482</v>
@@ -5568,13 +5634,197 @@
         <v>493</v>
       </c>
       <c r="E148" t="s">
-        <v>35</v>
+        <v>345</v>
       </c>
       <c r="F148" t="s">
         <v>492</v>
       </c>
       <c r="G148" t="s">
         <v>494</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>499</v>
+      </c>
+      <c r="B149" t="s">
+        <v>50</v>
+      </c>
+      <c r="C149" t="s">
+        <v>51</v>
+      </c>
+      <c r="D149" t="s">
+        <v>421</v>
+      </c>
+      <c r="E149" t="s">
+        <v>345</v>
+      </c>
+      <c r="F149" t="s">
+        <v>501</v>
+      </c>
+      <c r="G149" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>499</v>
+      </c>
+      <c r="B150" t="s">
+        <v>50</v>
+      </c>
+      <c r="C150" t="s">
+        <v>51</v>
+      </c>
+      <c r="D150" t="s">
+        <v>502</v>
+      </c>
+      <c r="E150" t="s">
+        <v>345</v>
+      </c>
+      <c r="F150" t="s">
+        <v>503</v>
+      </c>
+      <c r="G150" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>499</v>
+      </c>
+      <c r="B151" t="s">
+        <v>50</v>
+      </c>
+      <c r="C151" t="s">
+        <v>51</v>
+      </c>
+      <c r="D151" t="s">
+        <v>505</v>
+      </c>
+      <c r="E151" t="s">
+        <v>35</v>
+      </c>
+      <c r="F151" t="s">
+        <v>503</v>
+      </c>
+      <c r="G151" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>507</v>
+      </c>
+      <c r="B152" t="s">
+        <v>98</v>
+      </c>
+      <c r="C152" t="s">
+        <v>99</v>
+      </c>
+      <c r="D152" t="s">
+        <v>508</v>
+      </c>
+      <c r="E152" t="s">
+        <v>345</v>
+      </c>
+      <c r="F152" t="s">
+        <v>510</v>
+      </c>
+      <c r="G152" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>507</v>
+      </c>
+      <c r="B153" t="s">
+        <v>98</v>
+      </c>
+      <c r="C153" t="s">
+        <v>99</v>
+      </c>
+      <c r="D153" t="s">
+        <v>354</v>
+      </c>
+      <c r="E153" t="s">
+        <v>345</v>
+      </c>
+      <c r="F153" t="s">
+        <v>512</v>
+      </c>
+      <c r="G153" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>513</v>
+      </c>
+      <c r="B154" t="s">
+        <v>98</v>
+      </c>
+      <c r="C154" t="s">
+        <v>99</v>
+      </c>
+      <c r="D154" t="s">
+        <v>514</v>
+      </c>
+      <c r="E154" t="s">
+        <v>345</v>
+      </c>
+      <c r="F154" t="s">
+        <v>512</v>
+      </c>
+      <c r="G154" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>513</v>
+      </c>
+      <c r="B155" t="s">
+        <v>98</v>
+      </c>
+      <c r="C155" t="s">
+        <v>99</v>
+      </c>
+      <c r="D155" t="s">
+        <v>189</v>
+      </c>
+      <c r="E155" t="s">
+        <v>345</v>
+      </c>
+      <c r="F155" t="s">
+        <v>517</v>
+      </c>
+      <c r="G155" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>513</v>
+      </c>
+      <c r="B156" t="s">
+        <v>98</v>
+      </c>
+      <c r="C156" t="s">
+        <v>99</v>
+      </c>
+      <c r="D156" t="s">
+        <v>519</v>
+      </c>
+      <c r="E156" t="s">
+        <v>35</v>
+      </c>
+      <c r="F156" t="s">
+        <v>517</v>
+      </c>
+      <c r="G156" t="s">
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Discount in Receipt only if(discount > 0)
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="548">
   <si>
     <t>S No</t>
   </si>
@@ -1634,6 +1634,33 @@
   </si>
   <si>
     <t>XX1512157</t>
+  </si>
+  <si>
+    <t>16-Dec-2020 19:25</t>
+  </si>
+  <si>
+    <t>GuestCust 33</t>
+  </si>
+  <si>
+    <t>XX1612158</t>
+  </si>
+  <si>
+    <t>16-Dec-2020 19:28</t>
+  </si>
+  <si>
+    <t>GuestCust 34</t>
+  </si>
+  <si>
+    <t>XX1612159</t>
+  </si>
+  <si>
+    <t>GuestCust 35</t>
+  </si>
+  <si>
+    <t>130.0</t>
+  </si>
+  <si>
+    <t>XX1612160</t>
   </si>
 </sst>
 </file>
@@ -2158,7 +2185,7 @@
         <v>155</v>
       </c>
       <c r="D2" t="n">
-        <v>117.0</v>
+        <v>116.0</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>157</v>
@@ -2181,7 +2208,7 @@
         <v>200</v>
       </c>
       <c r="D3" t="n">
-        <v>402.0</v>
+        <v>399.0</v>
       </c>
       <c r="F3" t="s">
         <v>164</v>
@@ -2241,7 +2268,7 @@
         <v>150.0</v>
       </c>
       <c r="D6" t="n">
-        <v>99.0</v>
+        <v>97.0</v>
       </c>
       <c r="F6" t="s">
         <v>496</v>
@@ -6040,6 +6067,75 @@
       </c>
       <c r="G163" t="s">
         <v>506</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>539</v>
+      </c>
+      <c r="B164" t="s">
+        <v>540</v>
+      </c>
+      <c r="C164" t="s">
+        <v>322</v>
+      </c>
+      <c r="D164" t="s">
+        <v>333</v>
+      </c>
+      <c r="E164" t="s">
+        <v>35</v>
+      </c>
+      <c r="F164" t="s">
+        <v>541</v>
+      </c>
+      <c r="G164" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>542</v>
+      </c>
+      <c r="B165" t="s">
+        <v>543</v>
+      </c>
+      <c r="C165" t="s">
+        <v>322</v>
+      </c>
+      <c r="D165" t="s">
+        <v>189</v>
+      </c>
+      <c r="E165" t="s">
+        <v>35</v>
+      </c>
+      <c r="F165" t="s">
+        <v>544</v>
+      </c>
+      <c r="G165" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>542</v>
+      </c>
+      <c r="B166" t="s">
+        <v>545</v>
+      </c>
+      <c r="C166" t="s">
+        <v>322</v>
+      </c>
+      <c r="D166" t="s">
+        <v>546</v>
+      </c>
+      <c r="E166" t="s">
+        <v>35</v>
+      </c>
+      <c r="F166" t="s">
+        <v>547</v>
+      </c>
+      <c r="G166" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Currency Calc Initial Fix
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="551">
   <si>
     <t>S No</t>
   </si>
@@ -1661,6 +1661,15 @@
   </si>
   <si>
     <t>XX1612160</t>
+  </si>
+  <si>
+    <t>17-Dec-2020 13:11</t>
+  </si>
+  <si>
+    <t>GuestCust 36</t>
+  </si>
+  <si>
+    <t>XX1712161</t>
   </si>
 </sst>
 </file>
@@ -2185,7 +2194,7 @@
         <v>155</v>
       </c>
       <c r="D2" t="n">
-        <v>116.0</v>
+        <v>115.0</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>157</v>
@@ -6135,6 +6144,29 @@
         <v>547</v>
       </c>
       <c r="G166" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>548</v>
+      </c>
+      <c r="B167" t="s">
+        <v>549</v>
+      </c>
+      <c r="C167" t="s">
+        <v>322</v>
+      </c>
+      <c r="D167" t="s">
+        <v>203</v>
+      </c>
+      <c r="E167" t="s">
+        <v>35</v>
+      </c>
+      <c r="F167" t="s">
+        <v>550</v>
+      </c>
+      <c r="G167" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>